<commit_message>
Reduce CBS concentration below solubility limit.
</commit_message>
<xml_diff>
--- a/examples/CAII-CBS/caii.xlsx
+++ b/examples/CAII-CBS/caii.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,7 +413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20191202a1.itc</t>
+          <t>20191203a1.itc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20191202a2.itc</t>
+          <t>20191203a2.itc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20191202a3.itc</t>
+          <t>20191203a3.itc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20191202a4.itc</t>
+          <t>20191203a4.itc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -609,34 +609,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20191202a5.itc</t>
+          <t>20191203a5.itc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CBS into CAII 1</t>
+          <t>buffer into CAII 1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Plates Quick.setup</t>
+          <t>Plates Clean.setup</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaWaterWater.inj</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Onesite</t>
+          <t>Control</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3311005429401354</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -658,34 +658,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20191202a6.itc</t>
+          <t>20191203a6.itc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CBS into CAII 1</t>
+          <t>buffer into CAII 1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Plates Quick.setup</t>
+          <t>Plates Clean.setup</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaWaterWater.inj</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Onesite</t>
+          <t>Control</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5231503635202742</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -707,7 +707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20191202a7.itc</t>
+          <t>20191203a7.itc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -731,10 +731,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8575285224941928</v>
+        <v>0.3311005429401354</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -756,12 +756,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20191202a8.itc</t>
+          <t>20191203a8.itc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CBS into CAII 1</t>
+          <t>CBS into CAII 2</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G9" t="n">
         <v>0.3311005429401354</v>
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20191202a9.itc</t>
+          <t>20191203a9.itc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="G10" t="n">
         <v>0.5231503635202742</v>
@@ -854,12 +854,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20191202a10.itc</t>
+          <t>20191203a10.itc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CBS into CAII 1</t>
+          <t>CBS into CAII 2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -878,10 +878,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8575285224941928</v>
+        <v>0.5231503635202742</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -903,34 +903,34 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20191202a11.itc</t>
+          <t>20191203a11.itc</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>final cleaning water titration</t>
+          <t>CBS into CAII 1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>water5inj.inj</t>
+          <t>ChoderaHSA.inj</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Control</t>
+          <t>Onesite</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.8575285224941928</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -952,34 +952,34 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20191202a12.itc</t>
+          <t>20191203a12.itc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>final water into water test 1</t>
+          <t>CBS into CAII 2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ChoderaWaterWater.inj</t>
+          <t>ChoderaHSA.inj</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Control</t>
+          <t>Onesite</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.8575285224941928</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1001,34 +1001,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20191202a13.itc</t>
+          <t>20191203a13.itc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>final water into water test 2</t>
+          <t>CBS into CAII 1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ChoderaWaterWater.inj</t>
+          <t>ChoderaHSA.inj</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Control</t>
+          <t>Onesite</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.3311005429401354</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1044,6 +1044,398 @@
       <c r="K14" t="inlineStr">
         <is>
           <t>Plate1, A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>20191203a14.itc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CBS into CAII 2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3311005429401354</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Plate1, C4</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Plate1, D4</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Plate1, C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>20191203a15.itc</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CBS into CAII 1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.5231503635202742</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Plate1, E4</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Plate1, F4</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Plate1, E4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>20191203a16.itc</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CBS into CAII 2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5231503635202742</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Plate1, G4</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Plate1, H4</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Plate1, G4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>20191203a17.itc</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CBS into CAII 1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.8575285224941928</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Plate1, A5</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Plate1, B5</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Plate1, A5</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>20191203a18.itc</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CBS into CAII 2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.8575285224941928</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Plate1, C5</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Plate1, D5</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Plate1, C5</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>20191203a19.itc</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>final cleaning water titration</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Plates Clean.setup</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>water5inj.inj</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Plate1, E5</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Plate1, F5</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Plate1, E5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20191203a20.itc</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>final water into water test 1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Plates Clean.setup</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ChoderaWaterWater.inj</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Plate1, G5</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Plate1, H5</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Plate1, G5</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20191203a21.itc</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>final water into water test 2</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Plates Clean.setup</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ChoderaWaterWater.inj</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Plate1, A6</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Plate1, B6</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Plate1, A6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for hCAII experiment
</commit_message>
<xml_diff>
--- a/examples/CAII-CBS/caii.xlsx
+++ b/examples/CAII-CBS/caii.xlsx
@@ -413,7 +413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20191203a1.itc</t>
+          <t>20191204a1.itc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20191203a2.itc</t>
+          <t>20191204a2.itc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20191203a3.itc</t>
+          <t>20191204a3.itc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20191203a4.itc</t>
+          <t>20191204a4.itc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -609,7 +609,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20191203a5.itc</t>
+          <t>20191204a5.itc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -658,7 +658,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20191203a6.itc</t>
+          <t>20191204a6.itc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -707,7 +707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20191203a7.itc</t>
+          <t>20191204a7.itc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20191203a8.itc</t>
+          <t>20191204a8.itc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20191203a9.itc</t>
+          <t>20191204a9.itc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20191203a10.itc</t>
+          <t>20191204a10.itc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -903,7 +903,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20191203a11.itc</t>
+          <t>20191204a11.itc</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20191203a12.itc</t>
+          <t>20191204a12.itc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1001,7 +1001,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20191203a13.itc</t>
+          <t>20191204a13.itc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1050,7 +1050,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20191203a14.itc</t>
+          <t>20191204a14.itc</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1099,7 +1099,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20191203a15.itc</t>
+          <t>20191204a15.itc</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20191203a16.itc</t>
+          <t>20191204a16.itc</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1197,7 +1197,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20191203a17.itc</t>
+          <t>20191204a17.itc</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1246,7 +1246,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20191203a18.itc</t>
+          <t>20191204a18.itc</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1295,7 +1295,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20191203a19.itc</t>
+          <t>20191204a19.itc</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1344,7 +1344,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20191203a20.itc</t>
+          <t>20191204a20.itc</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1393,7 +1393,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20191203a21.itc</t>
+          <t>20191204a21.itc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">

</xml_diff>